<commit_message>
refactor: Question1.class duplicated values into containers.
</commit_message>
<xml_diff>
--- a/Processed output.xlsx
+++ b/Processed output.xlsx
@@ -1,18 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent>
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vigneshj\Desktop\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr documentId="13_ncr:1_{0750E1C2-784F-4BB7-8AAB-DA3558760F6F}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="512" activeTab="1"/>
+    <workbookView tabRatio="512" windowHeight="13140" windowWidth="24240" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
   </bookViews>
   <sheets>
-    <sheet name="Employee data" sheetId="1" r:id="rId1"/>
-    <sheet name="Output" sheetId="5" r:id="rId2"/>
-    <sheet name="Processed output" sheetId="6" r:id="rId3"/>
+    <sheet name="Employee data" r:id="rId1" sheetId="1"/>
+    <sheet name="Output" r:id="rId2" sheetId="5"/>
+    <sheet name="Processed output" r:id="rId6" sheetId="6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Employee data'!$A$1:$D$475</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'Employee data'!$A$1:$D$475</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -98,10 +104,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
+    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -165,49 +171,49 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
   </cellStyleXfs>
   <cellXfs count="12">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="3" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="2" fontId="3" numFmtId="3" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="2" fontId="3" numFmtId="165" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="2" numFmtId="3" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="2" numFmtId="165" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="15" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="2" numFmtId="15" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="2" numFmtId="44" xfId="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="2" fontId="3" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
-    <cellStyle name="Walutowy" xfId="1" builtinId="4"/>
+    <cellStyle builtinId="4" name="Currency" xfId="1"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -220,14 +226,14 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motyw pakietu Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Pakiet Office">
+    <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -260,9 +266,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Pakiet Office">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin panose="020F0302020204030204" typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -295,9 +301,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -330,9 +353,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Pakiet Office">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -385,7 +425,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -394,13 +434,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -410,7 +450,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -419,7 +459,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -428,7 +468,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -438,12 +478,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -474,7 +514,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -493,7 +533,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -505,18 +545,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D475"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E475"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0" zoomScaleNormal="100"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="4" width="4.0" collapsed="false"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="3" width="15.7109375" collapsed="false"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="3" width="8.5703125" collapsed="false"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="4" width="10.85546875" collapsed="false"/>
+    <col min="5" max="16384" style="3" width="9.140625" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -7171,25 +7211,23 @@
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
-  <pageSetup firstPageNumber="0" fitToWidth="0" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageMargins bottom="1" footer="0" header="0" left="0.75" right="0.75" top="1"/>
+  <pageSetup firstPageNumber="0" fitToHeight="0" fitToWidth="0" orientation="landscape" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C327F8A8-B6D1-4FEA-A0AD-8A2B60477CE1}">
+  <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9" style="9"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="9" width="15.7109375" collapsed="false"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="9" width="17.42578125" collapsed="false"/>
+    <col min="3" max="16384" style="9" width="9.0" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -7315,30 +7353,25 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B18"/>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1">
       <c r="A1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -7346,7 +7379,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -7354,7 +7387,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -7362,7 +7395,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -7370,12 +7403,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7">
       <c r="A7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -7383,7 +7416,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -7391,7 +7424,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -7399,7 +7432,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -7407,7 +7440,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -7415,7 +7448,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -7423,7 +7456,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -7431,7 +7464,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16">
       <c r="A16" t="s">
         <v>2</v>
       </c>
@@ -7439,7 +7472,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17">
       <c r="A17" t="s">
         <v>3</v>
       </c>
@@ -7447,7 +7480,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -7456,6 +7489,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>